<commit_message>
Add ids to possible questions
</commit_message>
<xml_diff>
--- a/2022-01-16 Possible Questions Brainstorm.xlsx
+++ b/2022-01-16 Possible Questions Brainstorm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cooper/Projects/Personal/ios-trivia-react-native/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4267951-EB4D-704F-A430-B659123F445A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFAB60E-585D-FF48-931C-08545E0FE6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{AE7BDB45-B816-A545-97C3-B4FA7C1A2839}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="58">
   <si>
     <t>Prompt</t>
   </si>
@@ -99,9 +99,6 @@
     <t>https://www.theverge.com/2011/12/7/2585779/android-10th-anniversary-google-history-pie-oreo-nougat-cupcake</t>
   </si>
   <si>
-    <t>Unlike its biggest competitor, Android, which introduced widgets in its initial release in 2008, iOS didn't receive widgest until 2020.</t>
-  </si>
-  <si>
     <t>What was the original name for iOS?</t>
   </si>
   <si>
@@ -169,13 +166,55 @@
   </si>
   <si>
     <t>iOS 3</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>Unlike its biggest competitor, Android, which introduced widgets in its initial release in 2008, iOS didn't receive widgets until 2020.</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>cd047938-bb05-4de2-ba29-5167f1ac0a19</t>
+  </si>
+  <si>
+    <t>162bdc7f-a0f2-40bd-98f8-049f85ac94f6</t>
+  </si>
+  <si>
+    <t>bc561e51-0111-45b9-a9a6-73021f753eee</t>
+  </si>
+  <si>
+    <t>272aca63-4d7a-4a6a-afd2-6e5b6f23b563</t>
+  </si>
+  <si>
+    <t>04810b89-3a17-43c3-a3c7-8c796543eba9</t>
+  </si>
+  <si>
+    <t>8829a111-ef35-4395-be90-55669236eaf6</t>
+  </si>
+  <si>
+    <t>fd830e32-c539-446d-8fb1-bf56b6600492</t>
+  </si>
+  <si>
+    <t>643372e2-d080-4fdd-b8cc-9e4e3e681773</t>
+  </si>
+  <si>
+    <t>7541d979-f25b-45e7-9e2e-c75d883f8be6</t>
+  </si>
+  <si>
+    <t>6296ea7f-ff5b-470f-bb56-ab960ce02117</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -195,6 +234,13 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -221,7 +267,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -231,6 +277,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -546,302 +594,369 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C24FE9F3-BBEB-DE4D-B908-F119072BDD5C}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.1640625" customWidth="1"/>
-    <col min="2" max="2" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.1640625" customWidth="1"/>
+    <col min="3" max="3" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="22" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="J1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="J2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>8</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>9</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="J3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>16</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>19</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>20</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>39</v>
-      </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
         <v>40</v>
       </c>
       <c r="G5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" t="s">
         <v>9</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="C6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" t="s">
         <v>26</v>
       </c>
-      <c r="C6" t="s">
+      <c r="J6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" t="s">
         <v>42</v>
       </c>
-      <c r="D6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="H8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
         <v>14</v>
       </c>
-      <c r="F6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="E11" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="F11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="2" t="s">
+      <c r="I11" t="s">
         <v>37</v>
       </c>
-      <c r="H11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
+      <c r="J11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G11" r:id="rId1" display="https://www.lifewire.com/ios-versions-4147730" xr:uid="{6C3127BD-95D1-AA42-A436-C29A2483BCE8}"/>
+    <hyperlink ref="H11" r:id="rId1" display="https://www.lifewire.com/ios-versions-4147730" xr:uid="{6C3127BD-95D1-AA42-A436-C29A2483BCE8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Import questions from possible questions spreadsheet
</commit_message>
<xml_diff>
--- a/2022-01-16 Possible Questions Brainstorm.xlsx
+++ b/2022-01-16 Possible Questions Brainstorm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cooper/Projects/Personal/ios-trivia-react-native/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFAB60E-585D-FF48-931C-08545E0FE6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8BC0919-74A9-184C-8E3F-8D240E760F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{AE7BDB45-B816-A545-97C3-B4FA7C1A2839}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="15120" windowHeight="18880" xr2:uid="{AE7BDB45-B816-A545-97C3-B4FA7C1A2839}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -598,7 +598,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>